<commit_message>
Update - bon commande HURTEL ABRIS CONSO SN  LM 2023-24
</commit_message>
<xml_diff>
--- a/Documentation/Groupe/Revue 3/bon commande HURTEL ABRIS CONSO SN  LM 2023-24.xlsx
+++ b/Documentation/Groupe/Revue 3/bon commande HURTEL ABRIS CONSO SN  LM 2023-24.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joris HURTEL\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joris\Desktop\TP-Final-Gestion-de-la-conso\Documentation\Groupe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F052C320-2518-4577-A22C-26D07BE92E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8034141A-DEB3-4252-85D4-DD59F4ADD884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="85">
   <si>
     <t>Section :</t>
   </si>
@@ -228,22 +228,10 @@
     <t>https://www.lextronic.fr/capteur-de-courant-mikroe-2524-61861.html</t>
   </si>
   <si>
-    <t>https://store.arduino.cc/products/arduino-uno-rev3</t>
-  </si>
-  <si>
     <t>SKU A000066</t>
   </si>
   <si>
-    <t>ARDUINO</t>
-  </si>
-  <si>
-    <t>https://store.arduino.cc/products/portenta-hat-carrier?_gl=1*1smltca*_ga*NTQ3ODk0NDMuMTcwODA3MDA1MA..*_ga_NEXN8H46L5*MTcxMTA5MjExMS43LjEuMTcxMTA5MjU3NC4wLjAuOTQ0NDI2MzY5*_fplc*Sm4lMkJuVEhpak90aVo2N2JlWEJ5TFFrRU1qY1k1ZjRiRU4lMkI0a0N0REQzJTJCSUtnUjdjTkJ0R0YlMkZyJTJCJTJGQyUyRnN3YUhjbW03UW1kRHAxa1dxRU53NWJxTU16dkltQUJmRWIwTyUyRkhPVFliSnFDV1E1bmxHekFQNU10dThGOHFIQVNaZyUzRCUzRA..&amp;selectedStore=eu</t>
-  </si>
-  <si>
     <t xml:space="preserve">SKU ASX00049 </t>
-  </si>
-  <si>
-    <t>https://store.arduino.cc/products/portenta-h7</t>
   </si>
   <si>
     <t>SKU ABX00042</t>
@@ -330,6 +318,27 @@
       </rPr>
       <t xml:space="preserve"> 02</t>
     </r>
+  </si>
+  <si>
+    <t>https://fr.rs-online.com/web/p/arduino/2824023?searchId=ae991e20-3ef4-48bb-bcb9-45963d4ad131&amp;gb=s</t>
+  </si>
+  <si>
+    <t>https://fr.rs-online.com/web/p/arduino/7154081</t>
+  </si>
+  <si>
+    <t>TPX00132</t>
+  </si>
+  <si>
+    <t>https://fr.rs-online.com/web/p/arduino/2824018?searchId=448e3147-0f51-44ee-907f-68e534e6d4c1&amp;gb=s</t>
+  </si>
+  <si>
+    <t>TPX00094</t>
+  </si>
+  <si>
+    <t>https://fr.rs-online.com/web/p/shields-pour-arduino/2686968?searchId=81e00d62-9210-4e64-97d3-3a2b0de6d97d&amp;gb=s</t>
+  </si>
+  <si>
+    <t>https://fr.rs-online.com/web/p/arduino/2011441?searchId=b17b78cb-f531-4138-a0ab-b94a70044a93&amp;gb=s</t>
   </si>
 </sst>
 </file>
@@ -1019,6 +1028,79 @@
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="19" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1048,79 +1130,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="19" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1771,8 +1780,8 @@
   </sheetPr>
   <dimension ref="A1:X43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="S31" sqref="S31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1793,22 +1802,22 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F2" s="46" t="s">
-        <v>81</v>
-      </c>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="48"/>
+      <c r="F2" s="72" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="74"/>
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F3" s="49"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="51"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="77"/>
       <c r="L3" s="39"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
@@ -1818,15 +1827,15 @@
       <c r="T4" s="19"/>
     </row>
     <row r="5" spans="1:24" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="G5" s="53" t="s">
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="G5" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="53"/>
-      <c r="K5" s="53"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
       <c r="L5" s="10" t="s">
         <v>16</v>
       </c>
@@ -1848,15 +1857,15 @@
       <c r="B7" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="80"/>
       <c r="G7" s="30" t="s">
         <v>6</v>
       </c>
       <c r="H7" s="31"/>
-      <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="54"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="80"/>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
@@ -1886,15 +1895,15 @@
       <c r="B9" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" s="44"/>
-      <c r="G9" s="45" t="s">
-        <v>80</v>
-      </c>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
+      <c r="C9" s="70" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="70"/>
+      <c r="G9" s="71" t="s">
+        <v>76</v>
+      </c>
+      <c r="H9" s="71"/>
+      <c r="I9" s="71"/>
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
@@ -1924,16 +1933,16 @@
       <c r="X10" s="22"/>
     </row>
     <row r="11" spans="1:24" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="55" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="57" t="s">
+      <c r="B11" s="64" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="57"/>
+      <c r="G11" s="66"/>
       <c r="H11" s="24" t="s">
         <v>33</v>
       </c>
@@ -1970,16 +1979,16 @@
       <c r="A12">
         <v>1</v>
       </c>
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="60" t="s">
+      <c r="C12" s="68"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="60"/>
+      <c r="G12" s="69"/>
       <c r="H12" s="3">
         <v>33.520000000000003</v>
       </c>
@@ -2017,16 +2026,16 @@
       <c r="A13">
         <v>2</v>
       </c>
-      <c r="B13" s="61" t="s">
+      <c r="B13" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="63" t="s">
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="G13" s="63"/>
+      <c r="G13" s="50"/>
       <c r="H13" s="13">
         <v>38.090000000000003</v>
       </c>
@@ -2064,16 +2073,16 @@
       <c r="A14">
         <v>3</v>
       </c>
-      <c r="B14" s="64" t="s">
+      <c r="B14" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="65"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="66" t="s">
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="66"/>
+      <c r="G14" s="47"/>
       <c r="H14" s="1">
         <v>17.399999999999999</v>
       </c>
@@ -2111,16 +2120,16 @@
       <c r="A15">
         <v>4</v>
       </c>
-      <c r="B15" s="61" t="s">
+      <c r="B15" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="63">
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="50">
         <v>33457</v>
       </c>
-      <c r="G15" s="63"/>
+      <c r="G15" s="50"/>
       <c r="H15" s="13">
         <v>7.95</v>
       </c>
@@ -2158,16 +2167,16 @@
       <c r="A16">
         <v>5</v>
       </c>
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="65"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="66">
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="47">
         <v>31349</v>
       </c>
-      <c r="G16" s="66"/>
+      <c r="G16" s="47"/>
       <c r="H16" s="1">
         <v>12.5</v>
       </c>
@@ -2205,16 +2214,16 @@
       <c r="A17">
         <v>6</v>
       </c>
-      <c r="B17" s="61" t="s">
+      <c r="B17" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="62"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="62"/>
-      <c r="F17" s="63" t="s">
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="G17" s="63"/>
+      <c r="G17" s="50"/>
       <c r="H17" s="13">
         <v>12.6</v>
       </c>
@@ -2252,16 +2261,16 @@
       <c r="A18">
         <v>7</v>
       </c>
-      <c r="B18" s="64" t="s">
+      <c r="B18" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="65"/>
-      <c r="D18" s="65"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="66" t="s">
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="G18" s="66"/>
+      <c r="G18" s="47"/>
       <c r="H18" s="1">
         <v>24</v>
       </c>
@@ -2299,18 +2308,18 @@
       <c r="A19">
         <v>8</v>
       </c>
-      <c r="B19" s="61" t="s">
+      <c r="B19" s="62" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="62"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="63" t="s">
-        <v>57</v>
-      </c>
-      <c r="G19" s="63"/>
+      <c r="G19" s="50"/>
       <c r="H19" s="13">
-        <v>29.28</v>
+        <v>26.87</v>
       </c>
       <c r="I19" s="14">
         <v>1</v>
@@ -2320,10 +2329,10 @@
       </c>
       <c r="K19" s="35">
         <f t="shared" ref="K19:K35" si="0">H19*J19</f>
-        <v>29.28</v>
+        <v>26.87</v>
       </c>
       <c r="L19" s="17" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="M19" s="9"/>
       <c r="N19" s="32"/>
@@ -2344,18 +2353,18 @@
       <c r="A20">
         <v>9</v>
       </c>
-      <c r="B20" s="64" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="66" t="s">
-        <v>60</v>
-      </c>
-      <c r="G20" s="66"/>
+      <c r="B20" s="63" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="46"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" s="47"/>
       <c r="H20" s="1">
-        <v>47.58</v>
+        <v>47.94</v>
       </c>
       <c r="I20" s="2">
         <v>1</v>
@@ -2365,10 +2374,10 @@
       </c>
       <c r="K20" s="3">
         <f t="shared" si="0"/>
-        <v>47.58</v>
-      </c>
-      <c r="L20" s="6" t="s">
-        <v>58</v>
+        <v>47.94</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="M20" s="9"/>
       <c r="N20" s="33"/>
@@ -2389,18 +2398,18 @@
       <c r="A21">
         <v>10</v>
       </c>
-      <c r="B21" s="61" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="63" t="s">
-        <v>62</v>
-      </c>
-      <c r="G21" s="63"/>
+      <c r="B21" s="62" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" s="50"/>
       <c r="H21" s="13">
-        <v>108.7</v>
+        <v>118.8</v>
       </c>
       <c r="I21" s="14">
         <v>1</v>
@@ -2410,10 +2419,10 @@
       </c>
       <c r="K21" s="35">
         <f t="shared" si="0"/>
-        <v>108.7</v>
+        <v>118.8</v>
       </c>
       <c r="L21" s="17" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="M21" s="9"/>
       <c r="N21" s="32"/>
@@ -2434,16 +2443,16 @@
       <c r="A22">
         <v>11</v>
       </c>
-      <c r="B22" s="64" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="65"/>
-      <c r="D22" s="65"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="66" t="s">
-        <v>64</v>
-      </c>
-      <c r="G22" s="66"/>
+      <c r="B22" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="46"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="G22" s="47"/>
       <c r="H22" s="1">
         <v>5.0999999999999996</v>
       </c>
@@ -2479,16 +2488,16 @@
       <c r="A23">
         <v>12</v>
       </c>
-      <c r="B23" s="61" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="63" t="s">
-        <v>65</v>
-      </c>
-      <c r="G23" s="63"/>
+      <c r="B23" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" s="50"/>
       <c r="H23" s="13">
         <v>10.9</v>
       </c>
@@ -2521,16 +2530,16 @@
       <c r="A24">
         <v>13</v>
       </c>
-      <c r="B24" s="64" t="s">
-        <v>66</v>
-      </c>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="66">
+      <c r="B24" s="63" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="47">
         <v>4534</v>
       </c>
-      <c r="G24" s="66"/>
+      <c r="G24" s="47"/>
       <c r="H24" s="1">
         <v>4.9000000000000004</v>
       </c>
@@ -2563,16 +2572,16 @@
       <c r="A25">
         <v>14</v>
       </c>
-      <c r="B25" s="61" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" s="62"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="62"/>
-      <c r="F25" s="63" t="s">
-        <v>68</v>
-      </c>
-      <c r="G25" s="63"/>
+      <c r="B25" s="62" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="G25" s="50"/>
       <c r="H25" s="13">
         <v>4.5</v>
       </c>
@@ -2605,16 +2614,16 @@
       <c r="A26">
         <v>15</v>
       </c>
-      <c r="B26" s="64" t="s">
-        <v>69</v>
-      </c>
-      <c r="C26" s="65"/>
-      <c r="D26" s="65"/>
-      <c r="E26" s="65"/>
-      <c r="F26" s="66">
+      <c r="B26" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="47">
         <v>25932</v>
       </c>
-      <c r="G26" s="66"/>
+      <c r="G26" s="47"/>
       <c r="H26" s="1">
         <v>9.9</v>
       </c>
@@ -2648,16 +2657,16 @@
       <c r="A27">
         <v>16</v>
       </c>
-      <c r="B27" s="61" t="s">
-        <v>70</v>
-      </c>
-      <c r="C27" s="62"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="63" t="s">
-        <v>71</v>
-      </c>
-      <c r="G27" s="63"/>
+      <c r="B27" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" s="50"/>
       <c r="H27" s="13">
         <v>6.18</v>
       </c>
@@ -2672,7 +2681,7 @@
         <v>6.18</v>
       </c>
       <c r="L27" s="17" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="M27" s="9"/>
       <c r="N27" s="32"/>
@@ -2693,16 +2702,16 @@
       <c r="A28">
         <v>17</v>
       </c>
-      <c r="B28" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" s="65"/>
-      <c r="D28" s="65"/>
-      <c r="E28" s="65"/>
-      <c r="F28" s="66" t="s">
-        <v>74</v>
-      </c>
-      <c r="G28" s="66"/>
+      <c r="B28" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="46"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="G28" s="47"/>
       <c r="H28" s="1">
         <v>12.5</v>
       </c>
@@ -2738,16 +2747,16 @@
       <c r="A29">
         <v>18</v>
       </c>
-      <c r="B29" s="61" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" s="62"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="63" t="s">
-        <v>75</v>
-      </c>
-      <c r="G29" s="63"/>
+      <c r="B29" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="G29" s="50"/>
       <c r="H29" s="13">
         <v>15.5</v>
       </c>
@@ -2783,16 +2792,16 @@
       <c r="A30">
         <v>19</v>
       </c>
-      <c r="B30" s="64" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" s="65"/>
-      <c r="D30" s="65"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="66" t="s">
-        <v>78</v>
-      </c>
-      <c r="G30" s="66"/>
+      <c r="B30" s="63" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="G30" s="47"/>
       <c r="H30" s="1">
         <v>2.5499999999999998</v>
       </c>
@@ -2828,20 +2837,32 @@
       <c r="A31">
         <v>20</v>
       </c>
-      <c r="B31" s="67"/>
-      <c r="C31" s="62"/>
-      <c r="D31" s="62"/>
-      <c r="E31" s="62"/>
-      <c r="F31" s="63"/>
-      <c r="G31" s="63"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
+      <c r="B31" s="62" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="G31" s="50"/>
+      <c r="H31" s="13">
+        <v>6.59</v>
+      </c>
+      <c r="I31" s="14">
+        <v>1</v>
+      </c>
+      <c r="J31" s="14">
+        <v>1</v>
+      </c>
       <c r="K31" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L31" s="17"/>
+        <v>6.59</v>
+      </c>
+      <c r="L31" s="17" t="s">
+        <v>44</v>
+      </c>
       <c r="M31" s="9"/>
       <c r="N31" s="32"/>
       <c r="O31" s="12"/>
@@ -2861,20 +2882,32 @@
       <c r="A32">
         <v>21</v>
       </c>
-      <c r="B32" s="69"/>
-      <c r="C32" s="65"/>
-      <c r="D32" s="65"/>
-      <c r="E32" s="65"/>
-      <c r="F32" s="66"/>
-      <c r="G32" s="66"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
+      <c r="B32" s="63" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="46"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="G32" s="47"/>
+      <c r="H32" s="1">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="I32" s="2">
+        <v>1</v>
+      </c>
+      <c r="J32" s="2">
+        <v>1</v>
+      </c>
       <c r="K32" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L32" s="6"/>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="L32" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="M32" s="9"/>
       <c r="N32" s="33"/>
       <c r="O32" s="12"/>
@@ -2892,12 +2925,12 @@
       <c r="A33">
         <v>22</v>
       </c>
-      <c r="B33" s="67"/>
-      <c r="C33" s="62"/>
-      <c r="D33" s="62"/>
-      <c r="E33" s="62"/>
-      <c r="F33" s="63"/>
-      <c r="G33" s="63"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="50"/>
+      <c r="G33" s="50"/>
       <c r="H33" s="13"/>
       <c r="I33" s="14"/>
       <c r="J33" s="14"/>
@@ -2923,12 +2956,12 @@
       <c r="A34">
         <v>23</v>
       </c>
-      <c r="B34" s="69"/>
-      <c r="C34" s="65"/>
-      <c r="D34" s="65"/>
-      <c r="E34" s="65"/>
-      <c r="F34" s="66"/>
-      <c r="G34" s="66"/>
+      <c r="B34" s="45"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="47"/>
       <c r="H34" s="1"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
@@ -2954,12 +2987,12 @@
       <c r="A35">
         <v>24</v>
       </c>
-      <c r="B35" s="70"/>
-      <c r="C35" s="71"/>
-      <c r="D35" s="71"/>
-      <c r="E35" s="71"/>
-      <c r="F35" s="72"/>
-      <c r="G35" s="72"/>
+      <c r="B35" s="51"/>
+      <c r="C35" s="52"/>
+      <c r="D35" s="52"/>
+      <c r="E35" s="52"/>
+      <c r="F35" s="53"/>
+      <c r="G35" s="53"/>
       <c r="H35" s="15"/>
       <c r="I35" s="16"/>
       <c r="J35" s="16"/>
@@ -2982,20 +3015,20 @@
       <c r="X35" s="22"/>
     </row>
     <row r="36" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="73"/>
-      <c r="C36" s="74"/>
-      <c r="D36" s="74"/>
-      <c r="E36" s="75"/>
-      <c r="F36" s="76"/>
-      <c r="G36" s="77"/>
-      <c r="H36" s="78" t="s">
+      <c r="B36" s="54"/>
+      <c r="C36" s="55"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="58"/>
+      <c r="H36" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="I36" s="79"/>
-      <c r="J36" s="80"/>
+      <c r="I36" s="60"/>
+      <c r="J36" s="61"/>
       <c r="K36" s="37">
         <f>SUM(K12:K35)</f>
-        <v>262.69</v>
+        <v>287.52999999999997</v>
       </c>
       <c r="M36" s="9"/>
       <c r="N36" s="9"/>
@@ -3035,10 +3068,10 @@
       <c r="H38" s="9"/>
       <c r="I38" s="9"/>
       <c r="J38" s="9"/>
-      <c r="K38" s="68" t="s">
+      <c r="K38" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="L38" s="68"/>
+      <c r="L38" s="44"/>
       <c r="M38" s="9"/>
       <c r="N38" s="9"/>
       <c r="O38" s="9"/>
@@ -3175,6 +3208,55 @@
     <protectedRange algorithmName="SHA-512" hashValue="nhD1wKCtu4oniM6oqFxyMUl6vvbMrr6gE0g1CECeS1aGQqXBeL1KeE6et8XDvOUMXNDX0hWMaFZAF0++nsmhtw==" saltValue="9XCHs6crAD0LUZrbIMX22w==" spinCount="100000" sqref="S26:S31 S16:S20 S8:S13" name="Plage1"/>
   </protectedRanges>
   <mergeCells count="61">
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="F2:K3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="G5:K5"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="F31:G31"/>
     <mergeCell ref="K38:L38"/>
     <mergeCell ref="B32:E32"/>
     <mergeCell ref="F32:G32"/>
@@ -3187,55 +3269,6 @@
     <mergeCell ref="B36:E36"/>
     <mergeCell ref="F36:G36"/>
     <mergeCell ref="H36:J36"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="F2:K3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="G5:K5"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="I7:K7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B12" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
@@ -3246,7 +3279,7 @@
     <hyperlink ref="B17" r:id="rId6" xr:uid="{8E004100-38B0-4A76-ABCE-427CC535DFAF}"/>
     <hyperlink ref="B18" r:id="rId7" xr:uid="{FE7B64C1-B14F-4B90-8387-28574870797E}"/>
     <hyperlink ref="B19" r:id="rId8" xr:uid="{3FEFDDFC-DC30-4F71-9F49-51B3AC242E72}"/>
-    <hyperlink ref="B20" r:id="rId9" display="https://store.arduino.cc/products/portenta-hat-carrier?_gl=1*1smltca*_ga*NTQ3ODk0NDMuMTcwODA3MDA1MA..*_ga_NEXN8H46L5*MTcxMTA5MjExMS43LjEuMTcxMTA5MjU3NC4wLjAuOTQ0NDI2MzY5*_fplc*Sm4lMkJuVEhpak90aVo2N2JlWEJ5TFFrRU1qY1k1ZjRiRU4lMkI0a0N0REQzJTJCSUtnUjdjTkJ0R0YlMkZyJTJCJTJGQyUyRnN3YUhjbW03UW1kRHAxa1dxRU53NWJxTU16dkltQUJmRWIwTyUyRkhPVFliSnFDV1E1bmxHekFQNU10dThGOHFIQVNaZyUzRCUzRA..&amp;selectedStore=eu" xr:uid="{FFB2DF05-63B2-489B-ACBF-1FC164A8EAFB}"/>
+    <hyperlink ref="B20" r:id="rId9" xr:uid="{FFB2DF05-63B2-489B-ACBF-1FC164A8EAFB}"/>
     <hyperlink ref="B21" r:id="rId10" xr:uid="{4CCAB108-2083-498F-B565-BA25D781D3AE}"/>
     <hyperlink ref="B22" r:id="rId11" xr:uid="{BF8836E4-C88B-461A-99F3-05891DB3D762}"/>
     <hyperlink ref="B23" r:id="rId12" xr:uid="{E1984C21-B3B0-4BC0-B619-EFCF3369E68E}"/>
@@ -3258,17 +3291,19 @@
     <hyperlink ref="B29" r:id="rId18" xr:uid="{63D82767-2BD8-460D-BA7B-B0D816FA50E1}"/>
     <hyperlink ref="B30" r:id="rId19" xr:uid="{30A9BCAA-DF3D-4AFA-9158-C1246C0693D2}"/>
     <hyperlink ref="L5" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B31" r:id="rId21" xr:uid="{48977D4B-3E2F-4740-ABE8-7968B20F753F}"/>
+    <hyperlink ref="B32" r:id="rId22" xr:uid="{E982E780-3CEF-4A80-A02C-DB6291A0165F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="78" orientation="landscape" r:id="rId21"/>
-  <drawing r:id="rId22"/>
-  <legacyDrawing r:id="rId23"/>
+  <pageSetup paperSize="9" scale="78" orientation="landscape" r:id="rId23"/>
+  <drawing r:id="rId24"/>
+  <legacyDrawing r:id="rId25"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2049" r:id="rId24" name="Drop Down 1">
+            <control shapeId="2049" r:id="rId26" name="Drop Down 1">
               <controlPr locked="0" defaultSize="0" autoLine="0" autoPict="0" altText="Faites un choix">
                 <anchor>
                   <from>
@@ -3290,7 +3325,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2050" r:id="rId25" name="Drop Down 2">
+            <control shapeId="2050" r:id="rId27" name="Drop Down 2">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>

</xml_diff>